<commit_message>
adding plots to output & tidying processed data
</commit_message>
<xml_diff>
--- a/data/raw/investment/target_group.xlsx
+++ b/data/raw/investment/target_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulsharratt/Documents/Hertie/Semester 4/03 - Master's Thesis/thesis_stf/data/raw/investment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EB5FA2-330F-8B42-82C6-396EA848269D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D500EE6A-E78F-E64D-854A-7B0DE4A02048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4900" yWindow="23200" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4900" yWindow="22180" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1340,10 +1340,10 @@
     <hyperlink ref="B5" r:id="rId43" xr:uid="{4C79C552-7E91-2D47-A815-6305ADB1E1A4}"/>
     <hyperlink ref="B12" r:id="rId44" xr:uid="{65E995E3-4085-6D44-8192-A14EE61D0412}"/>
     <hyperlink ref="A12" r:id="rId45" xr:uid="{1C58387A-2F39-CB43-B62B-A0CC4245D259}"/>
-    <hyperlink ref="B17" r:id="rId46" xr:uid="{D5DA4F5F-EA1E-E341-BC31-01FD124D10C4}"/>
-    <hyperlink ref="A17" r:id="rId47" xr:uid="{5C6934F0-446E-0043-97D1-12CE7A7FF49C}"/>
-    <hyperlink ref="A2" r:id="rId48" xr:uid="{141980BA-8B11-C04F-9F07-E3C63BD9B6C5}"/>
-    <hyperlink ref="A26" r:id="rId49" display="https://gitlab.com/sequoia-pgp/" xr:uid="{952F1057-0D2A-7342-8BAD-55A3597B03F2}"/>
+    <hyperlink ref="A17" r:id="rId46" xr:uid="{5C6934F0-446E-0043-97D1-12CE7A7FF49C}"/>
+    <hyperlink ref="A2" r:id="rId47" xr:uid="{141980BA-8B11-C04F-9F07-E3C63BD9B6C5}"/>
+    <hyperlink ref="A26" r:id="rId48" display="https://gitlab.com/sequoia-pgp/" xr:uid="{952F1057-0D2A-7342-8BAD-55A3597B03F2}"/>
+    <hyperlink ref="B17" r:id="rId49" xr:uid="{09C9EB54-61EA-4245-AEA3-F74453B56353}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>